<commit_message>
continued work on BW analysis script
</commit_message>
<xml_diff>
--- a/data/BWdataset.xlsx
+++ b/data/BWdataset.xlsx
@@ -7626,7 +7626,9 @@
       </c>
       <c r="C181" s="36"/>
       <c r="D181" s="36"/>
-      <c r="E181" s="37"/>
+      <c r="E181" s="23">
+        <v>2.0</v>
+      </c>
       <c r="F181" s="16" t="s">
         <v>24</v>
       </c>

</xml_diff>